<commit_message>
Work on heli's project
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/uppsala_universitet/heli_hundred_lakes/metadata.xlsx
+++ b/metadata/excel/projects/uppsala_universitet/heli_hundred_lakes/metadata.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="460" windowWidth="27160" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="27160" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12543" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13251" uniqueCount="1179">
   <si>
     <t>Country</t>
   </si>
@@ -3655,6 +3655,12 @@
   </si>
   <si>
     <t>hundred_lakes_fung</t>
+  </si>
+  <si>
+    <t>~/SIFES/raw/projects/uppsala_universitet/</t>
+  </si>
+  <si>
+    <t>heli_hundred_lakes/</t>
   </si>
 </sst>
 </file>
@@ -4383,10 +4389,10 @@
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5087,7 +5093,7 @@
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="AB13" sqref="AB13"/>
+      <selection pane="bottomLeft" activeCell="I363" sqref="I363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5099,9 +5105,9 @@
     <col min="5" max="5" width="27.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="10" customWidth="1"/>
     <col min="7" max="7" width="21" style="25" customWidth="1"/>
-    <col min="8" max="8" width="33.1640625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="45.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="42" style="25" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="26" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="25" customWidth="1"/>
     <col min="11" max="11" width="33.33203125" style="47" customWidth="1"/>
     <col min="12" max="12" width="32" style="47" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
@@ -5194,7 +5200,7 @@
       <c r="Y1" s="29"/>
       <c r="Z1" s="15"/>
       <c r="AA1" s="46"/>
-      <c r="AB1" s="81"/>
+      <c r="AB1" s="80"/>
       <c r="AC1" s="65"/>
       <c r="AD1" s="65"/>
       <c r="AE1" s="65"/>
@@ -5217,24 +5223,24 @@
       <c r="AX1" s="4"/>
       <c r="AY1" s="4"/>
       <c r="AZ1" s="9"/>
-      <c r="BB1" s="80" t="s">
+      <c r="BB1" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="BC1" s="80"/>
-      <c r="BD1" s="80"/>
-      <c r="BE1" s="80"/>
-      <c r="BG1" s="80" t="s">
+      <c r="BC1" s="81"/>
+      <c r="BD1" s="81"/>
+      <c r="BE1" s="81"/>
+      <c r="BG1" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" s="80"/>
-      <c r="BI1" s="80"/>
-      <c r="BJ1" s="80"/>
-      <c r="BK1" s="80"/>
-      <c r="BL1" s="80"/>
-      <c r="BN1" s="80" t="s">
+      <c r="BH1" s="81"/>
+      <c r="BI1" s="81"/>
+      <c r="BJ1" s="81"/>
+      <c r="BK1" s="81"/>
+      <c r="BL1" s="81"/>
+      <c r="BN1" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" s="80"/>
+      <c r="BO1" s="81"/>
       <c r="BQ1" s="7" t="s">
         <v>67</v>
       </c>
@@ -5474,6 +5480,12 @@
       </c>
       <c r="G3" s="25" t="s">
         <v>1167</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>1178</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>445</v>
@@ -5640,6 +5652,12 @@
       <c r="G4" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H4" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J4" s="25" t="s">
         <v>446</v>
       </c>
@@ -5805,6 +5823,12 @@
       <c r="G5" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H5" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J5" s="25" t="s">
         <v>447</v>
       </c>
@@ -5970,6 +5994,12 @@
       <c r="G6" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H6" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J6" s="25" t="s">
         <v>448</v>
       </c>
@@ -6135,6 +6165,12 @@
       <c r="G7" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H7" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J7" s="25" t="s">
         <v>449</v>
       </c>
@@ -6300,6 +6336,12 @@
       <c r="G8" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H8" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J8" s="25" t="s">
         <v>450</v>
       </c>
@@ -6465,6 +6507,12 @@
       <c r="G9" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H9" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J9" s="25" t="s">
         <v>451</v>
       </c>
@@ -6630,6 +6678,12 @@
       <c r="G10" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H10" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J10" s="25" t="s">
         <v>452</v>
       </c>
@@ -6795,6 +6849,12 @@
       <c r="G11" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H11" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J11" s="25" t="s">
         <v>453</v>
       </c>
@@ -6960,6 +7020,12 @@
       <c r="G12" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H12" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J12" s="25" t="s">
         <v>454</v>
       </c>
@@ -7125,6 +7191,12 @@
       <c r="G13" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H13" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J13" s="25" t="s">
         <v>455</v>
       </c>
@@ -7290,6 +7362,12 @@
       <c r="G14" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H14" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J14" s="25" t="s">
         <v>456</v>
       </c>
@@ -7455,6 +7533,12 @@
       <c r="G15" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H15" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J15" s="25" t="s">
         <v>457</v>
       </c>
@@ -7620,6 +7704,12 @@
       <c r="G16" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H16" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J16" s="25" t="s">
         <v>458</v>
       </c>
@@ -7785,6 +7875,12 @@
       <c r="G17" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H17" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J17" s="25" t="s">
         <v>459</v>
       </c>
@@ -7950,6 +8046,12 @@
       <c r="G18" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H18" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J18" s="25" t="s">
         <v>460</v>
       </c>
@@ -8115,6 +8217,12 @@
       <c r="G19" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H19" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J19" s="25" t="s">
         <v>461</v>
       </c>
@@ -8280,6 +8388,12 @@
       <c r="G20" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H20" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J20" s="25" t="s">
         <v>462</v>
       </c>
@@ -8445,6 +8559,12 @@
       <c r="G21" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H21" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J21" s="25" t="s">
         <v>463</v>
       </c>
@@ -8610,6 +8730,12 @@
       <c r="G22" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H22" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J22" s="25" t="s">
         <v>464</v>
       </c>
@@ -8775,6 +8901,12 @@
       <c r="G23" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H23" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J23" s="25" t="s">
         <v>465</v>
       </c>
@@ -8940,6 +9072,12 @@
       <c r="G24" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H24" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J24" s="25" t="s">
         <v>466</v>
       </c>
@@ -9105,6 +9243,12 @@
       <c r="G25" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H25" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J25" s="25" t="s">
         <v>467</v>
       </c>
@@ -9270,6 +9414,12 @@
       <c r="G26" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H26" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J26" s="25" t="s">
         <v>468</v>
       </c>
@@ -9435,6 +9585,12 @@
       <c r="G27" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H27" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J27" s="25" t="s">
         <v>469</v>
       </c>
@@ -9600,6 +9756,12 @@
       <c r="G28" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H28" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J28" s="25" t="s">
         <v>470</v>
       </c>
@@ -9765,6 +9927,12 @@
       <c r="G29" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H29" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J29" s="25" t="s">
         <v>471</v>
       </c>
@@ -9930,6 +10098,12 @@
       <c r="G30" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H30" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J30" s="25" t="s">
         <v>472</v>
       </c>
@@ -10095,6 +10269,12 @@
       <c r="G31" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H31" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J31" s="25" t="s">
         <v>473</v>
       </c>
@@ -10260,6 +10440,12 @@
       <c r="G32" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H32" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J32" s="25" t="s">
         <v>474</v>
       </c>
@@ -10425,6 +10611,12 @@
       <c r="G33" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H33" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I33" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J33" s="25" t="s">
         <v>475</v>
       </c>
@@ -10590,6 +10782,12 @@
       <c r="G34" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H34" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J34" s="25" t="s">
         <v>476</v>
       </c>
@@ -10756,6 +10954,12 @@
       <c r="G35" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H35" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J35" s="25" t="s">
         <v>477</v>
       </c>
@@ -10911,6 +11115,12 @@
       <c r="G36" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H36" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J36" s="25" t="s">
         <v>478</v>
       </c>
@@ -11055,6 +11265,12 @@
       <c r="G37" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H37" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J37" s="25" t="s">
         <v>479</v>
       </c>
@@ -11198,6 +11414,12 @@
       <c r="G38" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H38" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J38" s="25" t="s">
         <v>480</v>
       </c>
@@ -11341,6 +11563,12 @@
       <c r="G39" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H39" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J39" s="25" t="s">
         <v>481</v>
       </c>
@@ -11484,6 +11712,12 @@
       <c r="G40" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H40" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J40" s="25" t="s">
         <v>482</v>
       </c>
@@ -11627,6 +11861,12 @@
       <c r="G41" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H41" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J41" s="25" t="s">
         <v>483</v>
       </c>
@@ -11770,6 +12010,12 @@
       <c r="G42" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H42" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J42" s="25" t="s">
         <v>484</v>
       </c>
@@ -11909,6 +12155,12 @@
       <c r="G43" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H43" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J43" s="25" t="s">
         <v>485</v>
       </c>
@@ -12048,6 +12300,12 @@
       <c r="G44" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H44" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I44" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J44" s="25" t="s">
         <v>486</v>
       </c>
@@ -12184,6 +12442,12 @@
       <c r="G45" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H45" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J45" s="25" t="s">
         <v>487</v>
       </c>
@@ -12320,6 +12584,12 @@
       <c r="G46" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H46" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J46" s="25" t="s">
         <v>488</v>
       </c>
@@ -12456,6 +12726,12 @@
       <c r="G47" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H47" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I47" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J47" s="25" t="s">
         <v>489</v>
       </c>
@@ -12592,6 +12868,12 @@
       <c r="G48" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H48" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J48" s="25" t="s">
         <v>490</v>
       </c>
@@ -12728,6 +13010,12 @@
       <c r="G49" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H49" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I49" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J49" s="25" t="s">
         <v>491</v>
       </c>
@@ -12864,6 +13152,12 @@
       <c r="G50" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H50" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J50" s="25" t="s">
         <v>492</v>
       </c>
@@ -13000,6 +13294,12 @@
       <c r="G51" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H51" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I51" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J51" s="25" t="s">
         <v>493</v>
       </c>
@@ -13136,6 +13436,12 @@
       <c r="G52" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H52" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I52" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J52" s="25" t="s">
         <v>494</v>
       </c>
@@ -13272,6 +13578,12 @@
       <c r="G53" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H53" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J53" s="25" t="s">
         <v>495</v>
       </c>
@@ -13408,6 +13720,12 @@
       <c r="G54" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H54" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I54" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J54" s="25" t="s">
         <v>496</v>
       </c>
@@ -13544,6 +13862,12 @@
       <c r="G55" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H55" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I55" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J55" s="25" t="s">
         <v>497</v>
       </c>
@@ -13680,6 +14004,12 @@
       <c r="G56" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H56" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I56" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J56" s="25" t="s">
         <v>498</v>
       </c>
@@ -13816,6 +14146,12 @@
       <c r="G57" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H57" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J57" s="25" t="s">
         <v>499</v>
       </c>
@@ -13952,6 +14288,12 @@
       <c r="G58" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H58" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I58" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J58" s="25" t="s">
         <v>500</v>
       </c>
@@ -14088,6 +14430,12 @@
       <c r="G59" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H59" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I59" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J59" s="25" t="s">
         <v>501</v>
       </c>
@@ -14224,6 +14572,12 @@
       <c r="G60" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H60" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I60" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J60" s="25" t="s">
         <v>502</v>
       </c>
@@ -14360,6 +14714,12 @@
       <c r="G61" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H61" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I61" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J61" s="25" t="s">
         <v>503</v>
       </c>
@@ -14496,6 +14856,12 @@
       <c r="G62" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H62" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I62" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J62" s="25" t="s">
         <v>504</v>
       </c>
@@ -14632,6 +14998,12 @@
       <c r="G63" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H63" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I63" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J63" s="25" t="s">
         <v>505</v>
       </c>
@@ -14768,6 +15140,12 @@
       <c r="G64" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H64" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I64" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J64" s="25" t="s">
         <v>506</v>
       </c>
@@ -14904,6 +15282,12 @@
       <c r="G65" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H65" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I65" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J65" s="25" t="s">
         <v>507</v>
       </c>
@@ -15039,6 +15423,12 @@
       <c r="G66" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H66" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I66" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J66" s="25" t="s">
         <v>508</v>
       </c>
@@ -15174,6 +15564,12 @@
       <c r="G67" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H67" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I67" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J67" s="25" t="s">
         <v>509</v>
       </c>
@@ -15309,6 +15705,12 @@
       <c r="G68" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H68" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I68" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J68" s="25" t="s">
         <v>510</v>
       </c>
@@ -15444,6 +15846,12 @@
       <c r="G69" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H69" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I69" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J69" s="25" t="s">
         <v>511</v>
       </c>
@@ -15579,6 +15987,12 @@
       <c r="G70" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H70" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I70" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J70" s="25" t="s">
         <v>512</v>
       </c>
@@ -15714,6 +16128,12 @@
       <c r="G71" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H71" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I71" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J71" s="25" t="s">
         <v>513</v>
       </c>
@@ -15849,6 +16269,12 @@
       <c r="G72" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H72" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I72" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J72" s="25" t="s">
         <v>514</v>
       </c>
@@ -15984,6 +16410,12 @@
       <c r="G73" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H73" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I73" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J73" s="25" t="s">
         <v>515</v>
       </c>
@@ -16119,6 +16551,12 @@
       <c r="G74" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H74" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I74" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J74" s="25" t="s">
         <v>516</v>
       </c>
@@ -16254,6 +16692,12 @@
       <c r="G75" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H75" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I75" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J75" s="25" t="s">
         <v>517</v>
       </c>
@@ -16389,6 +16833,12 @@
       <c r="G76" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H76" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I76" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J76" s="25" t="s">
         <v>518</v>
       </c>
@@ -16524,6 +16974,12 @@
       <c r="G77" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H77" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I77" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J77" s="25" t="s">
         <v>519</v>
       </c>
@@ -16659,6 +17115,12 @@
       <c r="G78" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H78" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I78" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J78" s="25" t="s">
         <v>520</v>
       </c>
@@ -16794,6 +17256,12 @@
       <c r="G79" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H79" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I79" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J79" s="25" t="s">
         <v>521</v>
       </c>
@@ -16929,6 +17397,12 @@
       <c r="G80" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H80" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I80" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J80" s="25" t="s">
         <v>522</v>
       </c>
@@ -17064,6 +17538,12 @@
       <c r="G81" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H81" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I81" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J81" s="25" t="s">
         <v>523</v>
       </c>
@@ -17199,6 +17679,12 @@
       <c r="G82" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H82" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I82" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J82" s="25" t="s">
         <v>524</v>
       </c>
@@ -17334,6 +17820,12 @@
       <c r="G83" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H83" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I83" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J83" s="25" t="s">
         <v>525</v>
       </c>
@@ -17469,6 +17961,12 @@
       <c r="G84" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H84" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I84" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J84" s="25" t="s">
         <v>526</v>
       </c>
@@ -17604,6 +18102,12 @@
       <c r="G85" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H85" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I85" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J85" s="25" t="s">
         <v>527</v>
       </c>
@@ -17739,6 +18243,12 @@
       <c r="G86" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H86" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I86" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J86" s="25" t="s">
         <v>528</v>
       </c>
@@ -17874,6 +18384,12 @@
       <c r="G87" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H87" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I87" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J87" s="25" t="s">
         <v>529</v>
       </c>
@@ -18009,6 +18525,12 @@
       <c r="G88" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H88" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I88" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J88" s="25" t="s">
         <v>530</v>
       </c>
@@ -18144,6 +18666,12 @@
       <c r="G89" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H89" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I89" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J89" s="25" t="s">
         <v>531</v>
       </c>
@@ -18279,6 +18807,12 @@
       <c r="G90" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H90" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I90" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J90" s="25" t="s">
         <v>532</v>
       </c>
@@ -18414,6 +18948,12 @@
       <c r="G91" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H91" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I91" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J91" s="25" t="s">
         <v>533</v>
       </c>
@@ -18549,6 +19089,12 @@
       <c r="G92" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H92" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I92" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J92" s="25" t="s">
         <v>534</v>
       </c>
@@ -18684,6 +19230,12 @@
       <c r="G93" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H93" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I93" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J93" s="25" t="s">
         <v>535</v>
       </c>
@@ -18819,6 +19371,12 @@
       <c r="G94" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H94" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I94" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J94" s="25" t="s">
         <v>536</v>
       </c>
@@ -18954,6 +19512,12 @@
       <c r="G95" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H95" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I95" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J95" s="25" t="s">
         <v>537</v>
       </c>
@@ -19086,6 +19650,12 @@
       <c r="G96" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H96" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I96" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J96" s="25" t="s">
         <v>538</v>
       </c>
@@ -19213,6 +19783,12 @@
       <c r="G97" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H97" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I97" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J97" s="25" t="s">
         <v>539</v>
       </c>
@@ -19348,6 +19924,12 @@
       <c r="G98" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H98" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I98" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J98" s="25" t="s">
         <v>540</v>
       </c>
@@ -19483,6 +20065,12 @@
       <c r="G99" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H99" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I99" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J99" s="25" t="s">
         <v>541</v>
       </c>
@@ -19618,6 +20206,12 @@
       <c r="G100" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H100" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I100" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J100" s="25" t="s">
         <v>542</v>
       </c>
@@ -19753,6 +20347,12 @@
       <c r="G101" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H101" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I101" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J101" s="25" t="s">
         <v>543</v>
       </c>
@@ -19888,6 +20488,12 @@
       <c r="G102" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H102" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I102" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J102" s="25" t="s">
         <v>544</v>
       </c>
@@ -20023,6 +20629,12 @@
       <c r="G103" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H103" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I103" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J103" s="25" t="s">
         <v>545</v>
       </c>
@@ -20150,6 +20762,12 @@
       <c r="G104" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H104" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I104" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J104" s="25" t="s">
         <v>546</v>
       </c>
@@ -20285,6 +20903,12 @@
       <c r="G105" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H105" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I105" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J105" s="25" t="s">
         <v>547</v>
       </c>
@@ -20417,6 +21041,12 @@
       <c r="G106" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H106" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I106" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J106" s="25" t="s">
         <v>548</v>
       </c>
@@ -20541,6 +21171,12 @@
       <c r="G107" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H107" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I107" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J107" s="25" t="s">
         <v>549</v>
       </c>
@@ -20665,6 +21301,12 @@
       <c r="G108" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H108" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I108" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J108" s="25" t="s">
         <v>550</v>
       </c>
@@ -20789,6 +21431,12 @@
       <c r="G109" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H109" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I109" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J109" s="25" t="s">
         <v>551</v>
       </c>
@@ -20913,6 +21561,12 @@
       <c r="G110" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H110" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I110" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J110" s="25" t="s">
         <v>552</v>
       </c>
@@ -21037,6 +21691,12 @@
       <c r="G111" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H111" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I111" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J111" s="25" t="s">
         <v>553</v>
       </c>
@@ -21161,6 +21821,12 @@
       <c r="G112" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H112" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I112" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J112" s="25" t="s">
         <v>554</v>
       </c>
@@ -21285,6 +21951,12 @@
       <c r="G113" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H113" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I113" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J113" s="25" t="s">
         <v>555</v>
       </c>
@@ -21409,6 +22081,12 @@
       <c r="G114" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H114" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I114" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J114" s="25" t="s">
         <v>556</v>
       </c>
@@ -21533,6 +22211,12 @@
       <c r="G115" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H115" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I115" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J115" s="25" t="s">
         <v>557</v>
       </c>
@@ -21657,6 +22341,12 @@
       <c r="G116" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H116" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I116" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J116" s="25" t="s">
         <v>558</v>
       </c>
@@ -21781,6 +22471,12 @@
       <c r="G117" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H117" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I117" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J117" s="25" t="s">
         <v>559</v>
       </c>
@@ -21905,6 +22601,12 @@
       <c r="G118" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H118" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I118" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J118" s="25" t="s">
         <v>560</v>
       </c>
@@ -22029,6 +22731,12 @@
       <c r="G119" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H119" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I119" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J119" s="25" t="s">
         <v>561</v>
       </c>
@@ -22153,6 +22861,12 @@
       <c r="G120" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H120" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I120" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J120" s="25" t="s">
         <v>562</v>
       </c>
@@ -22277,6 +22991,12 @@
       <c r="G121" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H121" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I121" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J121" s="25" t="s">
         <v>563</v>
       </c>
@@ -22400,6 +23120,12 @@
       <c r="G122" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H122" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I122" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J122" s="25" t="s">
         <v>564</v>
       </c>
@@ -22523,6 +23249,12 @@
       <c r="G123" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H123" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I123" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J123" s="25" t="s">
         <v>565</v>
       </c>
@@ -22646,6 +23378,12 @@
       <c r="G124" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H124" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I124" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J124" s="25" t="s">
         <v>566</v>
       </c>
@@ -22769,6 +23507,12 @@
       <c r="G125" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H125" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I125" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J125" s="25" t="s">
         <v>567</v>
       </c>
@@ -22892,6 +23636,12 @@
       <c r="G126" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H126" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I126" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J126" s="25" t="s">
         <v>568</v>
       </c>
@@ -23015,6 +23765,12 @@
       <c r="G127" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H127" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I127" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J127" s="25" t="s">
         <v>569</v>
       </c>
@@ -23138,6 +23894,12 @@
       <c r="G128" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H128" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I128" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J128" s="25" t="s">
         <v>570</v>
       </c>
@@ -23261,6 +24023,12 @@
       <c r="G129" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H129" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I129" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J129" s="25" t="s">
         <v>571</v>
       </c>
@@ -23384,6 +24152,12 @@
       <c r="G130" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H130" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I130" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J130" s="25" t="s">
         <v>572</v>
       </c>
@@ -23507,6 +24281,12 @@
       <c r="G131" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H131" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I131" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J131" s="25" t="s">
         <v>573</v>
       </c>
@@ -23630,6 +24410,12 @@
       <c r="G132" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H132" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I132" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J132" s="25" t="s">
         <v>574</v>
       </c>
@@ -23753,6 +24539,12 @@
       <c r="G133" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H133" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I133" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J133" s="25" t="s">
         <v>575</v>
       </c>
@@ -23876,6 +24668,12 @@
       <c r="G134" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H134" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I134" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J134" s="25" t="s">
         <v>576</v>
       </c>
@@ -24004,6 +24802,12 @@
       <c r="G135" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H135" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I135" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J135" s="25" t="s">
         <v>577</v>
       </c>
@@ -24133,6 +24937,12 @@
       <c r="G136" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H136" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I136" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J136" s="25" t="s">
         <v>578</v>
       </c>
@@ -24262,6 +25072,12 @@
       <c r="G137" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H137" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I137" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J137" s="25" t="s">
         <v>579</v>
       </c>
@@ -24391,6 +25207,12 @@
       <c r="G138" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H138" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I138" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J138" s="25" t="s">
         <v>580</v>
       </c>
@@ -24520,6 +25342,12 @@
       <c r="G139" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H139" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I139" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J139" s="25" t="s">
         <v>581</v>
       </c>
@@ -24649,6 +25477,12 @@
       <c r="G140" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H140" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I140" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J140" s="25" t="s">
         <v>582</v>
       </c>
@@ -24778,6 +25612,12 @@
       <c r="G141" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H141" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I141" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J141" s="25" t="s">
         <v>583</v>
       </c>
@@ -24907,6 +25747,12 @@
       <c r="G142" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H142" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I142" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J142" s="25" t="s">
         <v>584</v>
       </c>
@@ -25036,6 +25882,12 @@
       <c r="G143" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H143" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I143" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J143" s="25" t="s">
         <v>585</v>
       </c>
@@ -25165,6 +26017,12 @@
       <c r="G144" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H144" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I144" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J144" s="25" t="s">
         <v>586</v>
       </c>
@@ -25294,6 +26152,12 @@
       <c r="G145" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H145" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I145" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J145" s="25" t="s">
         <v>587</v>
       </c>
@@ -25423,6 +26287,12 @@
       <c r="G146" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H146" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I146" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J146" s="25" t="s">
         <v>588</v>
       </c>
@@ -25552,6 +26422,12 @@
       <c r="G147" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H147" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I147" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J147" s="25" t="s">
         <v>589</v>
       </c>
@@ -25681,6 +26557,12 @@
       <c r="G148" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H148" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I148" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J148" s="25" t="s">
         <v>590</v>
       </c>
@@ -25810,6 +26692,12 @@
       <c r="G149" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H149" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I149" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J149" s="25" t="s">
         <v>591</v>
       </c>
@@ -25939,6 +26827,12 @@
       <c r="G150" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H150" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I150" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J150" s="25" t="s">
         <v>592</v>
       </c>
@@ -26068,6 +26962,12 @@
       <c r="G151" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H151" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I151" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J151" s="25" t="s">
         <v>593</v>
       </c>
@@ -26197,6 +27097,12 @@
       <c r="G152" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H152" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I152" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J152" s="25" t="s">
         <v>594</v>
       </c>
@@ -26326,6 +27232,12 @@
       <c r="G153" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H153" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I153" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J153" s="25" t="s">
         <v>595</v>
       </c>
@@ -26455,6 +27367,12 @@
       <c r="G154" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H154" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I154" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J154" s="25" t="s">
         <v>596</v>
       </c>
@@ -26584,6 +27502,12 @@
       <c r="G155" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H155" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I155" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J155" s="25" t="s">
         <v>597</v>
       </c>
@@ -26713,6 +27637,12 @@
       <c r="G156" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H156" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I156" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J156" s="25" t="s">
         <v>598</v>
       </c>
@@ -26842,6 +27772,12 @@
       <c r="G157" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H157" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I157" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J157" s="25" t="s">
         <v>599</v>
       </c>
@@ -26968,6 +27904,12 @@
       <c r="G158" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H158" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I158" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J158" s="25" t="s">
         <v>600</v>
       </c>
@@ -27094,6 +28036,12 @@
       <c r="G159" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H159" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I159" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J159" s="25" t="s">
         <v>601</v>
       </c>
@@ -27220,6 +28168,12 @@
       <c r="G160" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H160" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I160" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J160" s="25" t="s">
         <v>602</v>
       </c>
@@ -27346,6 +28300,12 @@
       <c r="G161" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H161" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I161" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J161" s="25" t="s">
         <v>603</v>
       </c>
@@ -27472,6 +28432,12 @@
       <c r="G162" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H162" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I162" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J162" s="25" t="s">
         <v>604</v>
       </c>
@@ -27598,6 +28564,12 @@
       <c r="G163" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H163" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I163" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J163" s="25" t="s">
         <v>605</v>
       </c>
@@ -27724,6 +28696,12 @@
       <c r="G164" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H164" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I164" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J164" s="25" t="s">
         <v>606</v>
       </c>
@@ -27850,6 +28828,12 @@
       <c r="G165" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H165" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I165" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J165" s="25" t="s">
         <v>607</v>
       </c>
@@ -27976,6 +28960,12 @@
       <c r="G166" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H166" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I166" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J166" s="25" t="s">
         <v>608</v>
       </c>
@@ -28102,6 +29092,12 @@
       <c r="G167" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H167" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I167" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J167" s="25" t="s">
         <v>609</v>
       </c>
@@ -28228,6 +29224,12 @@
       <c r="G168" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H168" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I168" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J168" s="25" t="s">
         <v>610</v>
       </c>
@@ -28354,6 +29356,12 @@
       <c r="G169" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H169" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I169" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J169" s="25" t="s">
         <v>611</v>
       </c>
@@ -28480,6 +29488,12 @@
       <c r="G170" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H170" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I170" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J170" s="25" t="s">
         <v>612</v>
       </c>
@@ -28606,6 +29620,12 @@
       <c r="G171" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H171" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I171" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J171" s="25" t="s">
         <v>613</v>
       </c>
@@ -28732,6 +29752,12 @@
       <c r="G172" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H172" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I172" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J172" s="25" t="s">
         <v>614</v>
       </c>
@@ -28858,6 +29884,12 @@
       <c r="G173" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H173" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I173" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J173" s="25" t="s">
         <v>615</v>
       </c>
@@ -28984,6 +30016,12 @@
       <c r="G174" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H174" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I174" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J174" s="25" t="s">
         <v>616</v>
       </c>
@@ -29110,6 +30148,12 @@
       <c r="G175" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H175" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I175" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J175" s="25" t="s">
         <v>617</v>
       </c>
@@ -29236,6 +30280,12 @@
       <c r="G176" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H176" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I176" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J176" s="25" t="s">
         <v>618</v>
       </c>
@@ -29362,6 +30412,12 @@
       <c r="G177" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H177" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I177" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J177" s="25" t="s">
         <v>619</v>
       </c>
@@ -29488,6 +30544,12 @@
       <c r="G178" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H178" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I178" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J178" s="25" t="s">
         <v>620</v>
       </c>
@@ -29614,6 +30676,12 @@
       <c r="G179" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H179" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I179" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J179" s="25" t="s">
         <v>621</v>
       </c>
@@ -29740,6 +30808,12 @@
       <c r="G180" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H180" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I180" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J180" s="25" t="s">
         <v>445</v>
       </c>
@@ -29863,6 +30937,12 @@
       <c r="G181" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H181" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I181" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J181" s="25" t="s">
         <v>446</v>
       </c>
@@ -29995,6 +31075,12 @@
       <c r="G182" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H182" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I182" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J182" s="25" t="s">
         <v>447</v>
       </c>
@@ -30127,6 +31213,12 @@
       <c r="G183" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H183" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I183" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J183" s="25" t="s">
         <v>448</v>
       </c>
@@ -30259,6 +31351,12 @@
       <c r="G184" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H184" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I184" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J184" s="25" t="s">
         <v>449</v>
       </c>
@@ -30391,6 +31489,12 @@
       <c r="G185" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H185" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I185" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J185" s="25" t="s">
         <v>450</v>
       </c>
@@ -30523,6 +31627,12 @@
       <c r="G186" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H186" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I186" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J186" s="25" t="s">
         <v>451</v>
       </c>
@@ -30655,6 +31765,12 @@
       <c r="G187" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H187" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I187" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J187" s="25" t="s">
         <v>452</v>
       </c>
@@ -30787,6 +31903,12 @@
       <c r="G188" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H188" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I188" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J188" s="25" t="s">
         <v>453</v>
       </c>
@@ -30919,6 +32041,12 @@
       <c r="G189" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H189" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I189" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J189" s="25" t="s">
         <v>454</v>
       </c>
@@ -31051,6 +32179,12 @@
       <c r="G190" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H190" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I190" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J190" s="25" t="s">
         <v>455</v>
       </c>
@@ -31183,6 +32317,12 @@
       <c r="G191" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H191" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I191" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J191" s="25" t="s">
         <v>456</v>
       </c>
@@ -31315,6 +32455,12 @@
       <c r="G192" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H192" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I192" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J192" s="25" t="s">
         <v>457</v>
       </c>
@@ -31447,6 +32593,12 @@
       <c r="G193" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H193" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I193" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J193" s="25" t="s">
         <v>458</v>
       </c>
@@ -31579,6 +32731,12 @@
       <c r="G194" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H194" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I194" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J194" s="25" t="s">
         <v>459</v>
       </c>
@@ -31711,6 +32869,12 @@
       <c r="G195" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H195" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I195" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J195" s="25" t="s">
         <v>460</v>
       </c>
@@ -31843,6 +33007,12 @@
       <c r="G196" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H196" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I196" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J196" s="25" t="s">
         <v>461</v>
       </c>
@@ -31975,6 +33145,12 @@
       <c r="G197" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H197" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I197" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J197" s="25" t="s">
         <v>462</v>
       </c>
@@ -32107,6 +33283,12 @@
       <c r="G198" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H198" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I198" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J198" s="25" t="s">
         <v>463</v>
       </c>
@@ -32239,6 +33421,12 @@
       <c r="G199" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H199" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I199" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J199" s="25" t="s">
         <v>464</v>
       </c>
@@ -32371,6 +33559,12 @@
       <c r="G200" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H200" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I200" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J200" s="25" t="s">
         <v>465</v>
       </c>
@@ -32503,6 +33697,12 @@
       <c r="G201" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H201" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I201" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J201" s="25" t="s">
         <v>466</v>
       </c>
@@ -32635,6 +33835,12 @@
       <c r="G202" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H202" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I202" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J202" s="25" t="s">
         <v>467</v>
       </c>
@@ -32767,6 +33973,12 @@
       <c r="G203" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H203" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I203" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J203" s="25" t="s">
         <v>468</v>
       </c>
@@ -32899,6 +34111,12 @@
       <c r="G204" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H204" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I204" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J204" s="25" t="s">
         <v>469</v>
       </c>
@@ -33031,6 +34249,12 @@
       <c r="G205" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H205" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I205" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J205" s="25" t="s">
         <v>470</v>
       </c>
@@ -33163,6 +34387,12 @@
       <c r="G206" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H206" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I206" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J206" s="25" t="s">
         <v>471</v>
       </c>
@@ -33295,6 +34525,12 @@
       <c r="G207" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H207" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I207" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J207" s="25" t="s">
         <v>472</v>
       </c>
@@ -33427,6 +34663,12 @@
       <c r="G208" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H208" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I208" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J208" s="25" t="s">
         <v>473</v>
       </c>
@@ -33559,6 +34801,12 @@
       <c r="G209" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H209" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I209" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J209" s="25" t="s">
         <v>474</v>
       </c>
@@ -33691,6 +34939,12 @@
       <c r="G210" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H210" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I210" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J210" s="25" t="s">
         <v>475</v>
       </c>
@@ -33823,6 +35077,12 @@
       <c r="G211" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H211" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I211" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J211" s="25" t="s">
         <v>476</v>
       </c>
@@ -33955,6 +35215,12 @@
       <c r="G212" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H212" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I212" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J212" s="25" t="s">
         <v>477</v>
       </c>
@@ -34087,6 +35353,12 @@
       <c r="G213" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H213" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I213" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J213" s="25" t="s">
         <v>478</v>
       </c>
@@ -34219,6 +35491,12 @@
       <c r="G214" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H214" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I214" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J214" s="25" t="s">
         <v>479</v>
       </c>
@@ -34351,6 +35629,12 @@
       <c r="G215" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H215" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I215" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J215" s="25" t="s">
         <v>480</v>
       </c>
@@ -34483,6 +35767,12 @@
       <c r="G216" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H216" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I216" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J216" s="25" t="s">
         <v>481</v>
       </c>
@@ -34615,6 +35905,12 @@
       <c r="G217" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H217" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I217" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J217" s="25" t="s">
         <v>482</v>
       </c>
@@ -34747,6 +36043,12 @@
       <c r="G218" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H218" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I218" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J218" s="25" t="s">
         <v>483</v>
       </c>
@@ -34879,6 +36181,12 @@
       <c r="G219" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H219" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I219" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J219" s="25" t="s">
         <v>484</v>
       </c>
@@ -35011,6 +36319,12 @@
       <c r="G220" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H220" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I220" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J220" s="25" t="s">
         <v>485</v>
       </c>
@@ -35143,6 +36457,12 @@
       <c r="G221" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H221" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I221" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J221" s="25" t="s">
         <v>486</v>
       </c>
@@ -35275,6 +36595,12 @@
       <c r="G222" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H222" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I222" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J222" s="25" t="s">
         <v>487</v>
       </c>
@@ -35407,6 +36733,12 @@
       <c r="G223" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H223" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I223" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J223" s="25" t="s">
         <v>488</v>
       </c>
@@ -35539,6 +36871,12 @@
       <c r="G224" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H224" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I224" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J224" s="25" t="s">
         <v>489</v>
       </c>
@@ -35671,6 +37009,12 @@
       <c r="G225" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H225" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I225" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J225" s="25" t="s">
         <v>490</v>
       </c>
@@ -35803,6 +37147,12 @@
       <c r="G226" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H226" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I226" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J226" s="25" t="s">
         <v>491</v>
       </c>
@@ -35935,6 +37285,12 @@
       <c r="G227" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H227" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I227" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J227" s="25" t="s">
         <v>492</v>
       </c>
@@ -36067,6 +37423,12 @@
       <c r="G228" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H228" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I228" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J228" s="25" t="s">
         <v>493</v>
       </c>
@@ -36199,6 +37561,12 @@
       <c r="G229" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H229" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I229" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J229" s="25" t="s">
         <v>494</v>
       </c>
@@ -36331,6 +37699,12 @@
       <c r="G230" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H230" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I230" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J230" s="25" t="s">
         <v>495</v>
       </c>
@@ -36463,6 +37837,12 @@
       <c r="G231" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H231" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I231" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J231" s="25" t="s">
         <v>496</v>
       </c>
@@ -36595,6 +37975,12 @@
       <c r="G232" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H232" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I232" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J232" s="25" t="s">
         <v>497</v>
       </c>
@@ -36727,6 +38113,12 @@
       <c r="G233" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H233" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I233" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J233" s="25" t="s">
         <v>498</v>
       </c>
@@ -36859,6 +38251,12 @@
       <c r="G234" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H234" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I234" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J234" s="25" t="s">
         <v>499</v>
       </c>
@@ -36991,6 +38389,12 @@
       <c r="G235" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H235" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I235" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J235" s="25" t="s">
         <v>500</v>
       </c>
@@ -37123,6 +38527,12 @@
       <c r="G236" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H236" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I236" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J236" s="25" t="s">
         <v>501</v>
       </c>
@@ -37255,6 +38665,12 @@
       <c r="G237" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H237" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I237" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J237" s="25" t="s">
         <v>502</v>
       </c>
@@ -37387,6 +38803,12 @@
       <c r="G238" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H238" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I238" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J238" s="25" t="s">
         <v>503</v>
       </c>
@@ -37519,6 +38941,12 @@
       <c r="G239" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H239" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I239" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J239" s="25" t="s">
         <v>504</v>
       </c>
@@ -37651,6 +39079,12 @@
       <c r="G240" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H240" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I240" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J240" s="25" t="s">
         <v>505</v>
       </c>
@@ -37783,6 +39217,12 @@
       <c r="G241" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H241" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I241" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J241" s="25" t="s">
         <v>506</v>
       </c>
@@ -37915,6 +39355,12 @@
       <c r="G242" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H242" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I242" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J242" s="25" t="s">
         <v>507</v>
       </c>
@@ -38047,6 +39493,12 @@
       <c r="G243" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H243" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I243" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J243" s="25" t="s">
         <v>508</v>
       </c>
@@ -38179,6 +39631,12 @@
       <c r="G244" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H244" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I244" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J244" s="25" t="s">
         <v>509</v>
       </c>
@@ -38311,6 +39769,12 @@
       <c r="G245" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H245" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I245" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J245" s="25" t="s">
         <v>510</v>
       </c>
@@ -38443,6 +39907,12 @@
       <c r="G246" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H246" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I246" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J246" s="25" t="s">
         <v>511</v>
       </c>
@@ -38575,6 +40045,12 @@
       <c r="G247" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H247" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I247" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J247" s="25" t="s">
         <v>512</v>
       </c>
@@ -38707,6 +40183,12 @@
       <c r="G248" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H248" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I248" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J248" s="25" t="s">
         <v>513</v>
       </c>
@@ -38839,6 +40321,12 @@
       <c r="G249" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H249" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I249" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J249" s="25" t="s">
         <v>514</v>
       </c>
@@ -38971,6 +40459,12 @@
       <c r="G250" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H250" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I250" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J250" s="25" t="s">
         <v>515</v>
       </c>
@@ -39103,6 +40597,12 @@
       <c r="G251" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H251" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I251" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J251" s="25" t="s">
         <v>516</v>
       </c>
@@ -39235,6 +40735,12 @@
       <c r="G252" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H252" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I252" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J252" s="25" t="s">
         <v>517</v>
       </c>
@@ -39367,6 +40873,12 @@
       <c r="G253" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H253" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I253" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J253" s="25" t="s">
         <v>518</v>
       </c>
@@ -39499,6 +41011,12 @@
       <c r="G254" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H254" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I254" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J254" s="25" t="s">
         <v>519</v>
       </c>
@@ -39631,6 +41149,12 @@
       <c r="G255" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H255" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I255" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J255" s="25" t="s">
         <v>520</v>
       </c>
@@ -39763,6 +41287,12 @@
       <c r="G256" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H256" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I256" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J256" s="25" t="s">
         <v>521</v>
       </c>
@@ -39895,6 +41425,12 @@
       <c r="G257" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H257" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I257" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J257" s="25" t="s">
         <v>522</v>
       </c>
@@ -40027,6 +41563,12 @@
       <c r="G258" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H258" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I258" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J258" s="25" t="s">
         <v>523</v>
       </c>
@@ -40159,6 +41701,12 @@
       <c r="G259" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H259" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I259" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J259" s="25" t="s">
         <v>524</v>
       </c>
@@ -40291,6 +41839,12 @@
       <c r="G260" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H260" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I260" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J260" s="25" t="s">
         <v>525</v>
       </c>
@@ -40423,6 +41977,12 @@
       <c r="G261" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H261" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I261" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J261" s="25" t="s">
         <v>526</v>
       </c>
@@ -40555,6 +42115,12 @@
       <c r="G262" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H262" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I262" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J262" s="25" t="s">
         <v>527</v>
       </c>
@@ -40687,6 +42253,12 @@
       <c r="G263" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H263" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I263" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J263" s="25" t="s">
         <v>528</v>
       </c>
@@ -40819,6 +42391,12 @@
       <c r="G264" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H264" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I264" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J264" s="25" t="s">
         <v>529</v>
       </c>
@@ -40951,6 +42529,12 @@
       <c r="G265" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H265" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I265" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J265" s="25" t="s">
         <v>530</v>
       </c>
@@ -41083,6 +42667,12 @@
       <c r="G266" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H266" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I266" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J266" s="25" t="s">
         <v>531</v>
       </c>
@@ -41215,6 +42805,12 @@
       <c r="G267" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H267" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I267" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J267" s="25" t="s">
         <v>532</v>
       </c>
@@ -41347,6 +42943,12 @@
       <c r="G268" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H268" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I268" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J268" s="25" t="s">
         <v>533</v>
       </c>
@@ -41479,6 +43081,12 @@
       <c r="G269" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H269" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I269" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J269" s="25" t="s">
         <v>534</v>
       </c>
@@ -41611,6 +43219,12 @@
       <c r="G270" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H270" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I270" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J270" s="25" t="s">
         <v>535</v>
       </c>
@@ -41743,6 +43357,12 @@
       <c r="G271" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H271" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I271" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J271" s="25" t="s">
         <v>536</v>
       </c>
@@ -41875,6 +43495,12 @@
       <c r="G272" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H272" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I272" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J272" s="25" t="s">
         <v>537</v>
       </c>
@@ -41998,6 +43624,12 @@
       <c r="G273" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H273" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I273" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J273" s="25" t="s">
         <v>538</v>
       </c>
@@ -42130,6 +43762,12 @@
       <c r="G274" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H274" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I274" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J274" s="25" t="s">
         <v>539</v>
       </c>
@@ -42262,6 +43900,12 @@
       <c r="G275" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H275" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I275" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J275" s="25" t="s">
         <v>540</v>
       </c>
@@ -42394,6 +44038,12 @@
       <c r="G276" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H276" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I276" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J276" s="25" t="s">
         <v>541</v>
       </c>
@@ -42526,6 +44176,12 @@
       <c r="G277" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H277" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I277" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J277" s="25" t="s">
         <v>542</v>
       </c>
@@ -42658,6 +44314,12 @@
       <c r="G278" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H278" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I278" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J278" s="25" t="s">
         <v>543</v>
       </c>
@@ -42790,6 +44452,12 @@
       <c r="G279" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H279" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I279" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J279" s="25" t="s">
         <v>544</v>
       </c>
@@ -42916,6 +44584,12 @@
       <c r="G280" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H280" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I280" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J280" s="25" t="s">
         <v>545</v>
       </c>
@@ -43048,6 +44722,12 @@
       <c r="G281" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H281" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I281" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J281" s="25" t="s">
         <v>546</v>
       </c>
@@ -43180,6 +44860,12 @@
       <c r="G282" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H282" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I282" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J282" s="25" t="s">
         <v>547</v>
       </c>
@@ -43305,6 +44991,12 @@
       <c r="G283" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H283" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I283" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J283" s="25" t="s">
         <v>548</v>
       </c>
@@ -43430,6 +45122,12 @@
       <c r="G284" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H284" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I284" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J284" s="25" t="s">
         <v>549</v>
       </c>
@@ -43555,6 +45253,12 @@
       <c r="G285" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H285" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I285" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J285" s="25" t="s">
         <v>550</v>
       </c>
@@ -43680,6 +45384,12 @@
       <c r="G286" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H286" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I286" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J286" s="25" t="s">
         <v>551</v>
       </c>
@@ -43805,6 +45515,12 @@
       <c r="G287" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H287" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I287" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J287" s="25" t="s">
         <v>552</v>
       </c>
@@ -43930,6 +45646,12 @@
       <c r="G288" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H288" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I288" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J288" s="25" t="s">
         <v>553</v>
       </c>
@@ -44055,6 +45777,12 @@
       <c r="G289" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H289" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I289" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J289" s="25" t="s">
         <v>554</v>
       </c>
@@ -44180,6 +45908,12 @@
       <c r="G290" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H290" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I290" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J290" s="25" t="s">
         <v>555</v>
       </c>
@@ -44305,6 +46039,12 @@
       <c r="G291" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H291" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I291" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J291" s="25" t="s">
         <v>556</v>
       </c>
@@ -44430,6 +46170,12 @@
       <c r="G292" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H292" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I292" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J292" s="25" t="s">
         <v>557</v>
       </c>
@@ -44555,6 +46301,12 @@
       <c r="G293" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H293" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I293" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J293" s="25" t="s">
         <v>558</v>
       </c>
@@ -44680,6 +46432,12 @@
       <c r="G294" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H294" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I294" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J294" s="25" t="s">
         <v>559</v>
       </c>
@@ -44805,6 +46563,12 @@
       <c r="G295" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H295" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I295" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J295" s="25" t="s">
         <v>560</v>
       </c>
@@ -44930,6 +46694,12 @@
       <c r="G296" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H296" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I296" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J296" s="25" t="s">
         <v>561</v>
       </c>
@@ -45055,6 +46825,12 @@
       <c r="G297" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H297" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I297" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J297" s="25" t="s">
         <v>562</v>
       </c>
@@ -45180,6 +46956,12 @@
       <c r="G298" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H298" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I298" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J298" s="25" t="s">
         <v>563</v>
       </c>
@@ -45305,6 +47087,12 @@
       <c r="G299" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H299" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I299" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J299" s="25" t="s">
         <v>564</v>
       </c>
@@ -45430,6 +47218,12 @@
       <c r="G300" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H300" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I300" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J300" s="25" t="s">
         <v>565</v>
       </c>
@@ -45555,6 +47349,12 @@
       <c r="G301" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H301" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I301" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J301" s="25" t="s">
         <v>566</v>
       </c>
@@ -45680,6 +47480,12 @@
       <c r="G302" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H302" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I302" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J302" s="25" t="s">
         <v>567</v>
       </c>
@@ -45805,6 +47611,12 @@
       <c r="G303" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H303" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I303" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J303" s="25" t="s">
         <v>568</v>
       </c>
@@ -45930,6 +47742,12 @@
       <c r="G304" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H304" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I304" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J304" s="25" t="s">
         <v>569</v>
       </c>
@@ -46055,6 +47873,12 @@
       <c r="G305" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H305" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I305" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J305" s="25" t="s">
         <v>570</v>
       </c>
@@ -46180,6 +48004,12 @@
       <c r="G306" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H306" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I306" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J306" s="25" t="s">
         <v>571</v>
       </c>
@@ -46305,6 +48135,12 @@
       <c r="G307" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H307" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I307" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J307" s="25" t="s">
         <v>572</v>
       </c>
@@ -46430,6 +48266,12 @@
       <c r="G308" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H308" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I308" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J308" s="25" t="s">
         <v>573</v>
       </c>
@@ -46555,6 +48397,12 @@
       <c r="G309" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H309" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I309" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J309" s="25" t="s">
         <v>574</v>
       </c>
@@ -46680,6 +48528,12 @@
       <c r="G310" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H310" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I310" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J310" s="25" t="s">
         <v>575</v>
       </c>
@@ -46805,6 +48659,12 @@
       <c r="G311" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H311" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I311" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J311" s="25" t="s">
         <v>576</v>
       </c>
@@ -46933,6 +48793,12 @@
       <c r="G312" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H312" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I312" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J312" s="25" t="s">
         <v>577</v>
       </c>
@@ -47061,6 +48927,12 @@
       <c r="G313" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H313" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I313" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J313" s="25" t="s">
         <v>578</v>
       </c>
@@ -47189,6 +49061,12 @@
       <c r="G314" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H314" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I314" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J314" s="25" t="s">
         <v>579</v>
       </c>
@@ -47317,6 +49195,12 @@
       <c r="G315" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H315" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I315" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J315" s="25" t="s">
         <v>580</v>
       </c>
@@ -47445,6 +49329,12 @@
       <c r="G316" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H316" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I316" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J316" s="25" t="s">
         <v>581</v>
       </c>
@@ -47573,6 +49463,12 @@
       <c r="G317" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H317" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I317" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J317" s="25" t="s">
         <v>582</v>
       </c>
@@ -47701,6 +49597,12 @@
       <c r="G318" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H318" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I318" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J318" s="25" t="s">
         <v>583</v>
       </c>
@@ -47829,6 +49731,12 @@
       <c r="G319" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H319" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I319" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J319" s="25" t="s">
         <v>584</v>
       </c>
@@ -47957,6 +49865,12 @@
       <c r="G320" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H320" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I320" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J320" s="25" t="s">
         <v>585</v>
       </c>
@@ -48085,6 +49999,12 @@
       <c r="G321" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H321" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I321" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J321" s="25" t="s">
         <v>586</v>
       </c>
@@ -48213,6 +50133,12 @@
       <c r="G322" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H322" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I322" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J322" s="25" t="s">
         <v>587</v>
       </c>
@@ -48341,6 +50267,12 @@
       <c r="G323" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H323" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I323" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J323" s="25" t="s">
         <v>588</v>
       </c>
@@ -48469,6 +50401,12 @@
       <c r="G324" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H324" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I324" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J324" s="25" t="s">
         <v>589</v>
       </c>
@@ -48597,6 +50535,12 @@
       <c r="G325" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H325" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I325" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J325" s="25" t="s">
         <v>590</v>
       </c>
@@ -48725,6 +50669,12 @@
       <c r="G326" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H326" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I326" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J326" s="25" t="s">
         <v>591</v>
       </c>
@@ -48853,6 +50803,12 @@
       <c r="G327" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H327" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I327" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J327" s="25" t="s">
         <v>592</v>
       </c>
@@ -48981,6 +50937,12 @@
       <c r="G328" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H328" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I328" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J328" s="25" t="s">
         <v>593</v>
       </c>
@@ -49109,6 +51071,12 @@
       <c r="G329" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H329" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I329" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J329" s="25" t="s">
         <v>594</v>
       </c>
@@ -49237,6 +51205,12 @@
       <c r="G330" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H330" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I330" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J330" s="25" t="s">
         <v>595</v>
       </c>
@@ -49365,6 +51339,12 @@
       <c r="G331" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H331" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I331" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J331" s="25" t="s">
         <v>596</v>
       </c>
@@ -49493,6 +51473,12 @@
       <c r="G332" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H332" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I332" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J332" s="25" t="s">
         <v>597</v>
       </c>
@@ -49621,6 +51607,12 @@
       <c r="G333" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H333" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I333" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J333" s="25" t="s">
         <v>598</v>
       </c>
@@ -49749,6 +51741,12 @@
       <c r="G334" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H334" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I334" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J334" s="25" t="s">
         <v>599</v>
       </c>
@@ -49877,6 +51875,12 @@
       <c r="G335" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H335" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I335" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J335" s="25" t="s">
         <v>600</v>
       </c>
@@ -50005,6 +52009,12 @@
       <c r="G336" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H336" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I336" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J336" s="25" t="s">
         <v>601</v>
       </c>
@@ -50133,6 +52143,12 @@
       <c r="G337" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H337" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I337" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J337" s="25" t="s">
         <v>602</v>
       </c>
@@ -50261,6 +52277,12 @@
       <c r="G338" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H338" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I338" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J338" s="25" t="s">
         <v>603</v>
       </c>
@@ -50389,6 +52411,12 @@
       <c r="G339" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H339" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I339" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J339" s="25" t="s">
         <v>604</v>
       </c>
@@ -50517,6 +52545,12 @@
       <c r="G340" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H340" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I340" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J340" s="25" t="s">
         <v>605</v>
       </c>
@@ -50645,6 +52679,12 @@
       <c r="G341" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H341" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I341" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J341" s="25" t="s">
         <v>606</v>
       </c>
@@ -50773,6 +52813,12 @@
       <c r="G342" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H342" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I342" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J342" s="25" t="s">
         <v>607</v>
       </c>
@@ -50901,6 +52947,12 @@
       <c r="G343" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H343" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I343" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J343" s="25" t="s">
         <v>608</v>
       </c>
@@ -51029,6 +53081,12 @@
       <c r="G344" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H344" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I344" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J344" s="25" t="s">
         <v>609</v>
       </c>
@@ -51157,6 +53215,12 @@
       <c r="G345" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H345" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I345" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J345" s="25" t="s">
         <v>610</v>
       </c>
@@ -51285,6 +53349,12 @@
       <c r="G346" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H346" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I346" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J346" s="25" t="s">
         <v>611</v>
       </c>
@@ -51413,6 +53483,12 @@
       <c r="G347" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H347" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I347" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J347" s="25" t="s">
         <v>612</v>
       </c>
@@ -51541,6 +53617,12 @@
       <c r="G348" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H348" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I348" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J348" s="25" t="s">
         <v>613</v>
       </c>
@@ -51669,6 +53751,12 @@
       <c r="G349" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H349" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I349" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J349" s="25" t="s">
         <v>614</v>
       </c>
@@ -51797,6 +53885,12 @@
       <c r="G350" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H350" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I350" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J350" s="25" t="s">
         <v>615</v>
       </c>
@@ -51925,6 +54019,12 @@
       <c r="G351" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H351" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I351" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J351" s="25" t="s">
         <v>616</v>
       </c>
@@ -52053,6 +54153,12 @@
       <c r="G352" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H352" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I352" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J352" s="25" t="s">
         <v>617</v>
       </c>
@@ -52181,6 +54287,12 @@
       <c r="G353" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H353" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I353" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J353" s="25" t="s">
         <v>618</v>
       </c>
@@ -52309,6 +54421,12 @@
       <c r="G354" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H354" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I354" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J354" s="25" t="s">
         <v>619</v>
       </c>
@@ -52437,6 +54555,12 @@
       <c r="G355" s="25" t="s">
         <v>1167</v>
       </c>
+      <c r="H355" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I355" s="26" t="s">
+        <v>1178</v>
+      </c>
       <c r="J355" s="25" t="s">
         <v>620</v>
       </c>
@@ -52564,6 +54688,12 @@
       </c>
       <c r="G356" s="25" t="s">
         <v>1167</v>
+      </c>
+      <c r="H356" s="25" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I356" s="26" t="s">
+        <v>1178</v>
       </c>
       <c r="J356" s="25" t="s">
         <v>621</v>
@@ -52685,9 +54815,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" topLeftCell="BX1">
+      <pane ySplit="2.03125" topLeftCell="A233" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="CH245" sqref="CH245"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -52705,19 +54845,9 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" topLeftCell="BX1">
-      <pane ySplit="2.03125" topLeftCell="A233" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="CH245" sqref="CH245"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>

</xml_diff>